<commit_message>
Using column numbers instead of headers because they keep changing.
</commit_message>
<xml_diff>
--- a/LIC Invoiced 100925.xlsx
+++ b/LIC Invoiced 100925.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lincolnoilco-my.sharepoint.com/personal/jhalstead_lincolnenergysolutions_com/Documents/Documents/UiPath/Penn Tank to FIIMP Transform/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{9F6B2CB4-C099-4F41-9035-FEA0032C7907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD57893B-405F-49E1-B57C-DCF521EE4B01}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{9F6B2CB4-C099-4F41-9035-FEA0032C7907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A61EF12-C01E-4AE3-AB20-A47E319F641B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{741C04F3-6E22-4253-96CD-A95B2E7C39AC}"/>
+    <workbookView xWindow="30270" yWindow="1470" windowWidth="21600" windowHeight="11235" xr2:uid="{741C04F3-6E22-4253-96CD-A95B2E7C39AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -666,9 +666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B890359-6D49-47E6-B297-AA7642F494D9}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2730,7 +2728,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4039A99C-F805-4877-AD38-FD456F45E7DF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF436112-6B5E-4557-A722-41F6BCE444DE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="urn:argus-direct-storage:queries"/>
   </ds:schemaRefs>

</xml_diff>